<commit_message>
Se adicionan las tacticas para cada requerimiento
</commit_message>
<xml_diff>
--- a/taller arq-2.xlsx
+++ b/taller arq-2.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas Salazar\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nelsonpinzon/Library/Mobile Documents/com~apple~CloudDocs/Documents/Especialización/Arquitectura de Software/Software-Architecture/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2741B2A8-AFAA-4319-B1D5-0F8E55EA0016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1CE6CAF-D865-6C4D-B11B-65BFAF9E0F56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{930C2BC0-64CF-D141-82C4-9B5BCF2C150D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="27740" windowHeight="17500" activeTab="6" xr2:uid="{930C2BC0-64CF-D141-82C4-9B5BCF2C150D}"/>
   </bookViews>
   <sheets>
     <sheet name="QA" sheetId="1" r:id="rId1"/>
     <sheet name="Ejemplos" sheetId="3" r:id="rId2"/>
-    <sheet name="constraint" sheetId="2" r:id="rId3"/>
+    <sheet name="R7" sheetId="8" r:id="rId3"/>
+    <sheet name="R5" sheetId="7" r:id="rId4"/>
+    <sheet name="R4" sheetId="4" r:id="rId5"/>
+    <sheet name="R1" sheetId="5" r:id="rId6"/>
+    <sheet name="R11" sheetId="6" r:id="rId7"/>
+    <sheet name="constraint" sheetId="2" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="73">
   <si>
     <t>Atributos Calidad</t>
   </si>
@@ -250,13 +255,16 @@
   </si>
   <si>
     <t>Lectura de datos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La combinación más común es combinar la prevención (disponibilidad) con la gestión de recursos (performance). </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -285,6 +293,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF232323"/>
+      <name val="CenturyGothic"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -300,7 +328,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -360,11 +388,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -395,6 +447,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -422,20 +483,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFE8EFF8"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -445,6 +527,1645 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>182160</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>53906</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>182520</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>54266</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="2" name="Entrada de lápiz 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{061E74F9-70B4-0444-9E5C-FB0697C153C2}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="182160" y="843120"/>
+            <a:ext cx="360" cy="360"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="2" name="Entrada de lápiz 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{061E74F9-70B4-0444-9E5C-FB0697C153C2}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="177840" y="838800"/>
+              <a:ext cx="9000" cy="9000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>182160</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>182520</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>360</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="2" name="Entrada de lápiz 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{791D2E67-9C64-4E46-AF94-E9B97AA2812E}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="182160" y="843120"/>
+            <a:ext cx="360" cy="360"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="2" name="Entrada de lápiz 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{061E74F9-70B4-0444-9E5C-FB0697C153C2}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="177840" y="838800"/>
+              <a:ext cx="9000" cy="9000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>101599</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>81898</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>631942</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45C67A14-6219-A543-9C7B-550C6779EAFC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2044699" y="907398"/>
+          <a:ext cx="10436343" cy="5556902"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectángulo 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{788EABF2-9421-D542-9386-7E97635CFD04}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4343400" y="1638300"/>
+          <a:ext cx="2781300" cy="3568700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="E8EFF8"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="E8EFF8"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-MX" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>178160</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>360</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="2" name="Entrada de lápiz 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{061E74F9-70B4-0444-9E5C-FB0697C153C2}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="182160" y="843120"/>
+            <a:ext cx="360" cy="360"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="2" name="Entrada de lápiz 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{061E74F9-70B4-0444-9E5C-FB0697C153C2}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="177840" y="838800"/>
+              <a:ext cx="9000" cy="9000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>139590</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>143933</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>435075</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E515D40C-3139-A242-9893-9B3A5AC6DFF8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1799057" y="1159933"/>
+          <a:ext cx="8592818" cy="5926667"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>372534</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>169333</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>118533</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>160867</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectángulo 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88DB29A6-F124-794B-B6FC-EE4EEC486E81}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2861734" y="1998133"/>
+          <a:ext cx="1405466" cy="3242734"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="E8EFF8"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="E8EFF8"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-MX" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>33868</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>186267</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>372534</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>135467</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Rectángulo 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53FBB342-0258-6E42-AD1B-F914EDEA168A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5842001" y="1811867"/>
+          <a:ext cx="2827866" cy="3810000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="E8EFF8"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="E8EFF8"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-MX" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>42334</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>17990</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>186265</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5559E46-4BAA-A049-B76E-C573874BF1AB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="872067" y="1254123"/>
+          <a:ext cx="7526866" cy="4435475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="E8EFF8"/>
+        </a:solidFill>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>465666</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>211666</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>143934</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectángulo 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B5515C6-A8A7-DF43-BD0B-E9F11D8B8C9B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2125133" y="2506133"/>
+          <a:ext cx="2235200" cy="2734734"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="E8EFF8"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="E8EFF8"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-MX" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>677333</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>186267</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>423333</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Rectángulo 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CBDCC99-09FD-FB49-A198-C163FEF67A0B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2336800" y="1625600"/>
+          <a:ext cx="2235200" cy="2734734"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="E8EFF8"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="E8EFF8"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-MX" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>401760</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>89987</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>402120</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>90347</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="6" name="Entrada de lápiz 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4CE72B3-0F6C-9F41-A9E8-9DC5EAF68C77}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="401760" y="1935720"/>
+            <a:ext cx="360" cy="360"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="6" name="Entrada de lápiz 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4CE72B3-0F6C-9F41-A9E8-9DC5EAF68C77}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="397440" y="1931400"/>
+              <a:ext cx="9000" cy="9000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>679693</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>166787</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>680053</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>167147</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="7" name="Entrada de lápiz 6">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66DB5221-B50A-FC49-B81E-718BD80A6E96}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="9806760" y="1402920"/>
+            <a:ext cx="360" cy="360"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="7" name="Entrada de lápiz 6">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66DB5221-B50A-FC49-B81E-718BD80A6E96}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9802440" y="1398600"/>
+              <a:ext cx="9000" cy="9000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>736600</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>8466</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>198438</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>198869</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Imagen 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3BCAD7F4-5BF4-E84D-9170-34735DCB9DAC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8991600" y="1254654"/>
+          <a:ext cx="5240338" cy="5349778"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>595313</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>166688</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>357188</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>103188</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Rectángulo 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6FC5989-59E5-BA40-9CBB-65DBD83D71C6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9675813" y="1619251"/>
+          <a:ext cx="3889375" cy="4889500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="E8EFF8"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="E8EFF8"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-MX" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>151870</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>111124</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>721275</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>87312</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Imagen 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3406602B-A97D-6348-B89B-C491119B5E5B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:srcRect t="1445"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10883370" y="2182812"/>
+          <a:ext cx="1394905" cy="3897313"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>722312</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>182562</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>177799</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>198438</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Imagen 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7465B07C-B3CC-2C4A-A526-B9C2213C7D81}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:srcRect l="7812" t="132075" r="1" b="-133962"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11453812" y="2254250"/>
+          <a:ext cx="280987" cy="428626"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>182160</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>53906</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>182520</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>54266</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="2" name="Entrada de lápiz 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33F4116E-67B6-F84F-BA54-7E3B90F50232}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="182160" y="843120"/>
+            <a:ext cx="360" cy="360"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="2" name="Entrada de lápiz 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{061E74F9-70B4-0444-9E5C-FB0697C153C2}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="177840" y="838800"/>
+              <a:ext cx="9000" cy="9000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>719667</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>22561</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>702732</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>140927</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73E7DCD6-7D42-5E47-9FAD-36503AEF6716}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1549400" y="852294"/>
+          <a:ext cx="8280399" cy="4791966"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>567267</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>67738</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>5</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectángulo 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE8C6AD1-19E7-4F4B-BE8A-AD548C6F6963}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3056467" y="1507071"/>
+          <a:ext cx="2506133" cy="3793067"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="E8EFF8"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="E8EFF8"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-MX" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>182160</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>182520</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>360</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="2" name="Entrada de lápiz 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E660344-66FD-F341-988B-7EFE2503FDA7}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="182160" y="843120"/>
+            <a:ext cx="360" cy="360"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="2" name="Entrada de lápiz 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{061E74F9-70B4-0444-9E5C-FB0697C153C2}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="177840" y="838800"/>
+              <a:ext cx="9000" cy="9000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>714347</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>194734</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>351365</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29B6FFE8-E46B-984A-ADA3-0EB103639AFB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1544080" y="821267"/>
+          <a:ext cx="7934352" cy="5101166"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>381001</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>177803</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>423337</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>177798</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectángulo 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52D1B495-96E8-1E46-9930-428E8C416810}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5359401" y="1413936"/>
+          <a:ext cx="2531536" cy="4267195"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="E8EFF8"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="E8EFF8"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-MX" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>338667</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>16930</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>177802</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Rectángulo 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F243D229-48E2-FA42-B348-4DA7EA106316}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2827867" y="2065863"/>
+          <a:ext cx="1303866" cy="1786472"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="E8EFF8"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="E8EFF8"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-MX" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/ink/ink1.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2022-02-06T15:41:55.038"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.025" units="cm"/>
+      <inkml:brushProperty name="height" value="0.025" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 0 24575,'0'0'0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink2.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2022-02-06T16:12:37.454"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.025" units="cm"/>
+      <inkml:brushProperty name="height" value="0.025" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 0 24575,'0'0'0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink3.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2022-02-06T15:41:55.038"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.025" units="cm"/>
+      <inkml:brushProperty name="height" value="0.025" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 0 24575,'0'0'0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink4.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2022-02-06T15:34:28.301"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.025" units="cm"/>
+      <inkml:brushProperty name="height" value="0.025" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 0 24575,'0'0'0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink5.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2022-02-06T15:36:10.952"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.025" units="cm"/>
+      <inkml:brushProperty name="height" value="0.025" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 1 24575,'0'0'0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink6.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2022-02-06T15:43:44.424"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.025" units="cm"/>
+      <inkml:brushProperty name="height" value="0.025" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 0 24575,'0'0'0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink7.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2022-02-06T15:53:25.310"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.025" units="cm"/>
+      <inkml:brushProperty name="height" value="0.025" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 0 24575,'0'0'0</inkml:trace>
+</inkml:ink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -746,21 +2467,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30A29C82-537D-0A41-8469-EA9B4533FFF4}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="2" max="2" width="18.875" customWidth="1"/>
-    <col min="3" max="3" width="53.875" customWidth="1"/>
-    <col min="4" max="4" width="38.125" customWidth="1"/>
-    <col min="5" max="5" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.83203125" customWidth="1"/>
+    <col min="3" max="3" width="53.83203125" customWidth="1"/>
+    <col min="4" max="4" width="38.1640625" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="13" t="s">
         <v>32</v>
       </c>
@@ -774,15 +2495,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1"/>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-    </row>
-    <row r="3" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+    </row>
+    <row r="3" spans="1:4" ht="51">
       <c r="A3" s="1" t="s">
         <v>33</v>
       </c>
@@ -796,7 +2517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="34">
       <c r="A4" s="1" t="s">
         <v>34</v>
       </c>
@@ -810,7 +2531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="51">
       <c r="A5" s="1" t="s">
         <v>35</v>
       </c>
@@ -824,7 +2545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="34">
       <c r="A6" s="1" t="s">
         <v>36</v>
       </c>
@@ -838,7 +2559,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="34">
       <c r="A7" s="1" t="s">
         <v>37</v>
       </c>
@@ -852,7 +2573,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="68">
       <c r="A8" s="1" t="s">
         <v>38</v>
       </c>
@@ -866,7 +2587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" s="11" customFormat="1" ht="34">
       <c r="A9" s="1" t="s">
         <v>39</v>
       </c>
@@ -880,21 +2601,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="26" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="23" t="s">
+    <row r="10" spans="1:4" s="17" customFormat="1" ht="51">
+      <c r="A10" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="25">
+      <c r="D10" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="11" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" s="11" customFormat="1" ht="51">
       <c r="A11" s="1" t="s">
         <v>41</v>
       </c>
@@ -908,21 +2629,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="26" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="23" t="s">
+    <row r="12" spans="1:4" s="17" customFormat="1" ht="34">
+      <c r="A12" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="25">
+      <c r="D12" s="16">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" s="11" customFormat="1" ht="34">
       <c r="A13" s="1" t="s">
         <v>45</v>
       </c>
@@ -936,7 +2657,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="34">
       <c r="A14" s="1" t="s">
         <v>47</v>
       </c>
@@ -950,11 +2671,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:7">
       <c r="E18" s="9"/>
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="5:7">
       <c r="F19" s="8"/>
     </row>
   </sheetData>
@@ -971,448 +2692,448 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1690F214-8FDE-4731-8FEA-1D59D092703F}">
   <dimension ref="A3:R20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10:R10"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="13.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.25" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" customWidth="1"/>
     <col min="8" max="9" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18">
       <c r="A3" s="13" t="s">
         <v>43</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="16" t="s">
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16" t="s">
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16" t="s">
+      <c r="K3" s="21"/>
+      <c r="L3" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="M3" s="16"/>
-      <c r="N3" s="16"/>
-      <c r="O3" s="16" t="s">
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="16"/>
-      <c r="Q3" s="16" t="s">
+      <c r="P3" s="21"/>
+      <c r="Q3" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="R3" s="16"/>
-    </row>
-    <row r="4" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R3" s="21"/>
+    </row>
+    <row r="4" spans="1:18" ht="15" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="17" t="s">
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17" t="s">
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17" t="s">
+      <c r="K4" s="22"/>
+      <c r="L4" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="M4" s="17"/>
-      <c r="N4" s="17"/>
-      <c r="O4" s="17" t="s">
+      <c r="M4" s="22"/>
+      <c r="N4" s="22"/>
+      <c r="O4" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="P4" s="17"/>
-      <c r="Q4" s="17" t="s">
+      <c r="P4" s="22"/>
+      <c r="Q4" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="R4" s="17"/>
-    </row>
-    <row r="5" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R4" s="22"/>
+    </row>
+    <row r="5" spans="1:18" ht="15.75" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="18" t="s">
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="H5" s="19"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="17" t="s">
+      <c r="H5" s="24"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17" t="s">
+      <c r="K5" s="22"/>
+      <c r="L5" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17" t="s">
+      <c r="M5" s="22"/>
+      <c r="N5" s="22"/>
+      <c r="O5" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="P5" s="17"/>
-      <c r="Q5" s="17" t="s">
+      <c r="P5" s="22"/>
+      <c r="Q5" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="R5" s="17"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R5" s="22"/>
+    </row>
+    <row r="6" spans="1:18" ht="17">
       <c r="A6" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17" t="s">
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17" t="s">
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17" t="s">
+      <c r="K6" s="22"/>
+      <c r="L6" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="17" t="s">
+      <c r="M6" s="22"/>
+      <c r="N6" s="22"/>
+      <c r="O6" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="P6" s="17"/>
-      <c r="Q6" s="17" t="s">
+      <c r="P6" s="22"/>
+      <c r="Q6" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="R6" s="17"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R6" s="22"/>
+    </row>
+    <row r="7" spans="1:18" ht="17">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17" t="s">
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17" t="s">
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17" t="s">
+      <c r="K7" s="22"/>
+      <c r="L7" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="M7" s="17"/>
-      <c r="N7" s="17"/>
-      <c r="O7" s="17" t="s">
+      <c r="M7" s="22"/>
+      <c r="N7" s="22"/>
+      <c r="O7" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="P7" s="17"/>
-      <c r="Q7" s="17" t="s">
+      <c r="P7" s="22"/>
+      <c r="Q7" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="R7" s="17"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R7" s="22"/>
+    </row>
+    <row r="8" spans="1:18" ht="17">
       <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17" t="s">
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17" t="s">
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17" t="s">
+      <c r="K8" s="22"/>
+      <c r="L8" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="M8" s="17"/>
-      <c r="N8" s="17"/>
-      <c r="O8" s="17" t="s">
+      <c r="M8" s="22"/>
+      <c r="N8" s="22"/>
+      <c r="O8" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="P8" s="17"/>
-      <c r="Q8" s="17" t="s">
+      <c r="P8" s="22"/>
+      <c r="Q8" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="R8" s="17"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="15"/>
-      <c r="N9" s="15"/>
-      <c r="O9" s="15"/>
-      <c r="P9" s="15"/>
-      <c r="Q9" s="15"/>
-      <c r="R9" s="15"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="15"/>
-      <c r="N10" s="15"/>
-      <c r="O10" s="15"/>
-      <c r="P10" s="15"/>
-      <c r="Q10" s="15"/>
-      <c r="R10" s="15"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="15"/>
-      <c r="P11" s="15"/>
-      <c r="Q11" s="15"/>
-      <c r="R11" s="15"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="15"/>
-      <c r="N12" s="15"/>
-      <c r="O12" s="15"/>
-      <c r="P12" s="15"/>
-      <c r="Q12" s="15"/>
-      <c r="R12" s="15"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="15"/>
-      <c r="M13" s="15"/>
-      <c r="N13" s="15"/>
-      <c r="O13" s="15"/>
-      <c r="P13" s="15"/>
-      <c r="Q13" s="15"/>
-      <c r="R13" s="15"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="15"/>
-      <c r="O14" s="15"/>
-      <c r="P14" s="15"/>
-      <c r="Q14" s="15"/>
-      <c r="R14" s="15"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="15"/>
-      <c r="M15" s="15"/>
-      <c r="N15" s="15"/>
-      <c r="O15" s="15"/>
-      <c r="P15" s="15"/>
-      <c r="Q15" s="15"/>
-      <c r="R15" s="15"/>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="15"/>
-      <c r="O16" s="15"/>
-      <c r="P16" s="15"/>
-      <c r="Q16" s="15"/>
-      <c r="R16" s="15"/>
-    </row>
-    <row r="17" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="15"/>
-      <c r="M17" s="15"/>
-      <c r="N17" s="15"/>
-      <c r="O17" s="15"/>
-      <c r="P17" s="15"/>
-      <c r="Q17" s="15"/>
-      <c r="R17" s="15"/>
-    </row>
-    <row r="18" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="15"/>
-      <c r="N18" s="15"/>
-      <c r="O18" s="15"/>
-      <c r="P18" s="15"/>
-      <c r="Q18" s="15"/>
-      <c r="R18" s="15"/>
-    </row>
-    <row r="19" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="15"/>
-      <c r="L19" s="15"/>
-      <c r="M19" s="15"/>
-      <c r="N19" s="15"/>
-      <c r="O19" s="15"/>
-      <c r="P19" s="15"/>
-      <c r="Q19" s="15"/>
-      <c r="R19" s="15"/>
-    </row>
-    <row r="20" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="15"/>
-      <c r="N20" s="15"/>
-      <c r="O20" s="15"/>
-      <c r="P20" s="15"/>
-      <c r="Q20" s="15"/>
-      <c r="R20" s="15"/>
+      <c r="R8" s="22"/>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="20"/>
+      <c r="O9" s="20"/>
+      <c r="P9" s="20"/>
+      <c r="Q9" s="20"/>
+      <c r="R9" s="20"/>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="20"/>
+      <c r="R10" s="20"/>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="20"/>
+      <c r="O11" s="20"/>
+      <c r="P11" s="20"/>
+      <c r="Q11" s="20"/>
+      <c r="R11" s="20"/>
+    </row>
+    <row r="12" spans="1:18">
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="20"/>
+      <c r="O12" s="20"/>
+      <c r="P12" s="20"/>
+      <c r="Q12" s="20"/>
+      <c r="R12" s="20"/>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="20"/>
+      <c r="M13" s="20"/>
+      <c r="N13" s="20"/>
+      <c r="O13" s="20"/>
+      <c r="P13" s="20"/>
+      <c r="Q13" s="20"/>
+      <c r="R13" s="20"/>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="20"/>
+      <c r="N14" s="20"/>
+      <c r="O14" s="20"/>
+      <c r="P14" s="20"/>
+      <c r="Q14" s="20"/>
+      <c r="R14" s="20"/>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
+      <c r="L15" s="20"/>
+      <c r="M15" s="20"/>
+      <c r="N15" s="20"/>
+      <c r="O15" s="20"/>
+      <c r="P15" s="20"/>
+      <c r="Q15" s="20"/>
+      <c r="R15" s="20"/>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
+      <c r="L16" s="20"/>
+      <c r="M16" s="20"/>
+      <c r="N16" s="20"/>
+      <c r="O16" s="20"/>
+      <c r="P16" s="20"/>
+      <c r="Q16" s="20"/>
+      <c r="R16" s="20"/>
+    </row>
+    <row r="17" spans="3:18">
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
+      <c r="L17" s="20"/>
+      <c r="M17" s="20"/>
+      <c r="N17" s="20"/>
+      <c r="O17" s="20"/>
+      <c r="P17" s="20"/>
+      <c r="Q17" s="20"/>
+      <c r="R17" s="20"/>
+    </row>
+    <row r="18" spans="3:18">
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="20"/>
+      <c r="N18" s="20"/>
+      <c r="O18" s="20"/>
+      <c r="P18" s="20"/>
+      <c r="Q18" s="20"/>
+      <c r="R18" s="20"/>
+    </row>
+    <row r="19" spans="3:18">
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
+      <c r="M19" s="20"/>
+      <c r="N19" s="20"/>
+      <c r="O19" s="20"/>
+      <c r="P19" s="20"/>
+      <c r="Q19" s="20"/>
+      <c r="R19" s="20"/>
+    </row>
+    <row r="20" spans="3:18">
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="20"/>
+      <c r="L20" s="20"/>
+      <c r="M20" s="20"/>
+      <c r="N20" s="20"/>
+      <c r="O20" s="20"/>
+      <c r="P20" s="20"/>
+      <c r="Q20" s="20"/>
+      <c r="R20" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="108">
@@ -1527,10 +3248,529 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0623F571-7076-6C4D-A578-FB633C755C8A}">
+  <dimension ref="B2:S3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:19">
+      <c r="B2" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
+      <c r="P2" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q2" s="21"/>
+      <c r="R2" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="S2" s="21"/>
+    </row>
+    <row r="3" spans="2:19" ht="17">
+      <c r="B3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
+      <c r="P3" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q3" s="22"/>
+      <c r="R3" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="S3" s="22"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="R2:S2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5323668-299A-E44E-B73D-B25EB7A1AA38}">
+  <dimension ref="B2:S3"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="2" spans="2:19">
+      <c r="B2" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="32"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="34"/>
+      <c r="M2" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" s="32"/>
+      <c r="O2" s="34"/>
+      <c r="P2" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q2" s="34"/>
+      <c r="R2" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="S2" s="34"/>
+    </row>
+    <row r="3" spans="2:19" ht="32" customHeight="1">
+      <c r="B3" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="I3" s="35"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="L3" s="37"/>
+      <c r="M3" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="N3" s="35"/>
+      <c r="O3" s="37"/>
+      <c r="P3" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q3" s="37"/>
+      <c r="R3" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="S3" s="37"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="R2:S2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25AEC900-B734-2B45-8076-F15E0B1D98AC}">
+  <dimension ref="B2:S5"/>
+  <sheetViews>
+    <sheetView topLeftCell="G9" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="2" spans="2:19">
+      <c r="B2" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
+      <c r="P2" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q2" s="21"/>
+      <c r="R2" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="S2" s="21"/>
+    </row>
+    <row r="3" spans="2:19" ht="17">
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
+      <c r="P3" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q3" s="22"/>
+      <c r="R3" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="S3" s="22"/>
+    </row>
+    <row r="5" spans="2:19">
+      <c r="B5" s="18" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="P3:Q3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96425BE7-A72B-4246-B6A1-769CCC3C96AE}">
+  <dimension ref="B2:S3"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="2" spans="2:19">
+      <c r="B2" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
+      <c r="P2" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q2" s="21"/>
+      <c r="R2" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="S2" s="21"/>
+    </row>
+    <row r="3" spans="2:19" ht="17">
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="I3" s="24"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
+      <c r="P3" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q3" s="22"/>
+      <c r="R3" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="S3" s="22"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="R2:S2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EA53071-05C6-0547-B91A-A90055EF607C}">
+  <dimension ref="B2:S3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="2" spans="2:19">
+      <c r="B2" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
+      <c r="P2" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q2" s="21"/>
+      <c r="R2" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="S2" s="21"/>
+    </row>
+    <row r="3" spans="2:19" ht="17">
+      <c r="B3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
+      <c r="P3" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q3" s="22"/>
+      <c r="R3" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="S3" s="22"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="R2:S2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A429A18-72F4-B848-95AD-CC18E605E895}">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -1538,12 +3778,12 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="45" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
@@ -1554,14 +3794,14 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:3">
+      <c r="A2" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-    </row>
-    <row r="3" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+    </row>
+    <row r="3" spans="1:3" ht="34">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1572,7 +3812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>

</xml_diff>